<commit_message>
HOD Column added in report
</commit_message>
<xml_diff>
--- a/App_Templates/PATemplate.xlsx
+++ b/App_Templates/PATemplate.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
   <si>
     <t>Advice No.</t>
   </si>
@@ -122,6 +122,12 @@
   </si>
   <si>
     <t>IRN REPORT</t>
+  </si>
+  <si>
+    <t>Supplier ID</t>
+  </si>
+  <si>
+    <t>Approved By</t>
   </si>
 </sst>
 </file>
@@ -516,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:AH7"/>
+  <dimension ref="B1:AJ7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+      <selection activeCell="AC6" sqref="AC6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -530,73 +536,74 @@
     <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.140625" customWidth="1"/>
     <col min="6" max="6" width="21.42578125" customWidth="1"/>
-    <col min="7" max="7" width="14" customWidth="1"/>
-    <col min="8" max="8" width="16.28515625" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.85546875" customWidth="1"/>
-    <col min="11" max="11" width="11.28515625" customWidth="1"/>
-    <col min="12" max="12" width="14.28515625" customWidth="1"/>
-    <col min="13" max="13" width="8.5703125" customWidth="1"/>
-    <col min="14" max="14" width="9.85546875" customWidth="1"/>
-    <col min="15" max="15" width="6.140625" customWidth="1"/>
-    <col min="16" max="16" width="12.7109375" customWidth="1"/>
-    <col min="17" max="17" width="11.140625" customWidth="1"/>
-    <col min="18" max="18" width="14.7109375" customWidth="1"/>
-    <col min="19" max="19" width="11.7109375" customWidth="1"/>
-    <col min="20" max="20" width="15.28515625" customWidth="1"/>
-    <col min="21" max="21" width="11.5703125" customWidth="1"/>
-    <col min="22" max="22" width="15.140625" customWidth="1"/>
-    <col min="23" max="23" width="11.28515625" customWidth="1"/>
-    <col min="24" max="24" width="14.85546875" customWidth="1"/>
-    <col min="25" max="25" width="19.7109375" customWidth="1"/>
-    <col min="26" max="26" width="15.140625" customWidth="1"/>
-    <col min="27" max="27" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="15" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="14" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="9" customWidth="1"/>
-    <col min="33" max="33" width="10.140625" customWidth="1"/>
-    <col min="34" max="34" width="8.85546875" customWidth="1"/>
+    <col min="7" max="8" width="14" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.85546875" customWidth="1"/>
+    <col min="12" max="12" width="11.28515625" customWidth="1"/>
+    <col min="13" max="13" width="14.28515625" customWidth="1"/>
+    <col min="14" max="14" width="8.5703125" customWidth="1"/>
+    <col min="15" max="15" width="9.85546875" customWidth="1"/>
+    <col min="16" max="16" width="6.140625" customWidth="1"/>
+    <col min="17" max="17" width="12.7109375" customWidth="1"/>
+    <col min="18" max="18" width="11.140625" customWidth="1"/>
+    <col min="19" max="19" width="14.7109375" customWidth="1"/>
+    <col min="20" max="20" width="11.7109375" customWidth="1"/>
+    <col min="21" max="21" width="15.28515625" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" customWidth="1"/>
+    <col min="23" max="23" width="15.140625" customWidth="1"/>
+    <col min="24" max="24" width="11.28515625" customWidth="1"/>
+    <col min="25" max="25" width="14.85546875" customWidth="1"/>
+    <col min="26" max="26" width="19.7109375" customWidth="1"/>
+    <col min="27" max="27" width="15.140625" customWidth="1"/>
+    <col min="28" max="28" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="9" customWidth="1"/>
+    <col min="35" max="35" width="10.140625" customWidth="1"/>
+    <col min="36" max="36" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="6"/>
       <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
     </row>
-    <row r="2" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
-      <c r="G2" s="6"/>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
     </row>
-    <row r="3" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>34</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
     </row>
-    <row r="4" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
     </row>
-    <row r="5" spans="2:34" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:36" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
@@ -616,88 +623,94 @@
         <v>13</v>
       </c>
       <c r="H5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="J5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="K5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="3" t="s">
+      <c r="L5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="M5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="M5" s="3" t="s">
+      <c r="N5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="N5" s="3" t="s">
+      <c r="O5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="O5" s="3" t="s">
+      <c r="P5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="P5" s="3" t="s">
+      <c r="Q5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="Q5" s="3" t="s">
+      <c r="R5" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="R5" s="3" t="s">
+      <c r="S5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="S5" s="3" t="s">
+      <c r="T5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="T5" s="3" t="s">
+      <c r="U5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="U5" s="3" t="s">
+      <c r="V5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="V5" s="3" t="s">
+      <c r="W5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="W5" s="3" t="s">
+      <c r="X5" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="X5" s="3" t="s">
+      <c r="Y5" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="Y5" s="3" t="s">
+      <c r="Z5" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="Z5" s="3" t="s">
+      <c r="AA5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="AA5" s="3" t="s">
+      <c r="AB5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="AB5" s="3" t="s">
+      <c r="AC5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="AC5" s="3" t="s">
+      <c r="AE5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="AD5" s="3" t="s">
+      <c r="AF5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="AE5" s="3" t="s">
+      <c r="AG5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="AF5" s="3" t="s">
+      <c r="AH5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="AG5" s="3" t="s">
+      <c r="AI5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="AH5" s="3" t="s">
+      <c r="AJ5" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -731,8 +744,10 @@
       <c r="AF6" s="2"/>
       <c r="AG6" s="2"/>
       <c r="AH6" s="2"/>
+      <c r="AI6" s="2"/>
+      <c r="AJ6" s="2"/>
     </row>
-    <row r="7" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -766,10 +781,12 @@
       <c r="AF7" s="2"/>
       <c r="AG7" s="2"/>
       <c r="AH7" s="2"/>
+      <c r="AI7" s="2"/>
+      <c r="AJ7" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="G1:I2"/>
+    <mergeCell ref="H1:J2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>